<commit_message>
Project work: udates, restructuring, add new features, etc
</commit_message>
<xml_diff>
--- a/SkylifterSourceFiles/Network_Information.xlsx
+++ b/SkylifterSourceFiles/Network_Information.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="121">
   <si>
     <t>Hostname</t>
   </si>
@@ -317,9 +317,6 @@
     <t>172.100.255.255</t>
   </si>
   <si>
-    <t>Services</t>
-  </si>
-  <si>
     <t>172.100.1.5</t>
   </si>
   <si>
@@ -335,9 +332,6 @@
     <t>ge-0/0/2</t>
   </si>
   <si>
-    <t>Customers</t>
-  </si>
-  <si>
     <t>192.170.11.1</t>
   </si>
   <si>
@@ -369,6 +363,33 @@
   </si>
   <si>
     <t>Area ID</t>
+  </si>
+  <si>
+    <t>to_Customers</t>
+  </si>
+  <si>
+    <t>to_Services</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>aggregation</t>
+  </si>
+  <si>
+    <t>core</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>loopback</t>
   </si>
 </sst>
 </file>
@@ -705,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -721,7 +742,7 @@
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,10 +765,13 @@
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -772,8 +796,11 @@
       <c r="H3">
         <v>49.100099999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -795,8 +822,11 @@
       <c r="G4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -818,31 +848,37 @@
       <c r="G5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E6">
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -867,8 +903,11 @@
       <c r="H8">
         <v>49.100099999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -890,8 +929,11 @@
       <c r="G9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -913,31 +955,37 @@
       <c r="G10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E11">
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -962,8 +1010,11 @@
       <c r="H13">
         <v>49.100099999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -985,8 +1036,11 @@
       <c r="G14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1008,31 +1062,37 @@
       <c r="G15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16">
         <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -1057,8 +1117,11 @@
       <c r="H18">
         <v>49.100099999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1080,8 +1143,11 @@
       <c r="G19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1103,31 +1169,37 @@
       <c r="G20" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21">
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E21">
         <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -1152,8 +1224,11 @@
       <c r="H23">
         <v>49.100200000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1175,8 +1250,11 @@
       <c r="G24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1198,31 +1276,37 @@
       <c r="G25" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C26">
         <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E26">
         <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1247,8 +1331,11 @@
       <c r="H28">
         <v>49.100200000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1270,8 +1357,11 @@
       <c r="G29" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>18</v>
       </c>
@@ -1293,31 +1383,37 @@
       <c r="G30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E31">
         <v>24</v>
       </c>
       <c r="F31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G31" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1342,8 +1438,11 @@
       <c r="H33">
         <v>49.100200000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1365,8 +1464,11 @@
       <c r="G34" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1388,31 +1490,37 @@
       <c r="G35" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36">
         <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E36">
         <v>24</v>
       </c>
       <c r="F36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G36" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -1437,8 +1545,11 @@
       <c r="H38">
         <v>49.100200000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>23</v>
       </c>
@@ -1460,8 +1571,11 @@
       <c r="G39" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>23</v>
       </c>
@@ -1483,31 +1597,37 @@
       <c r="G40" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41">
         <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E41">
         <v>24</v>
       </c>
       <c r="F41" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -1532,8 +1652,11 @@
       <c r="H43">
         <v>49.100200000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1555,8 +1678,11 @@
       <c r="G44" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -1578,31 +1704,37 @@
       <c r="G45" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C46">
         <v>25</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E46">
         <v>24</v>
       </c>
       <c r="F46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G46" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="I46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -1627,8 +1759,11 @@
       <c r="H48">
         <v>49.0002</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -1650,8 +1785,11 @@
       <c r="G49" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I49" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -1673,8 +1811,11 @@
       <c r="G50" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -1696,8 +1837,11 @@
       <c r="G51" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -1719,8 +1863,11 @@
       <c r="G52" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>24</v>
       </c>
@@ -1742,8 +1889,11 @@
       <c r="G53" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -1768,8 +1918,11 @@
       <c r="H55">
         <v>49.0002</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I55" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -1791,8 +1944,11 @@
       <c r="G56" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I56" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -1814,8 +1970,11 @@
       <c r="G57" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -1837,8 +1996,11 @@
       <c r="G58" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>25</v>
       </c>
@@ -1860,8 +2022,11 @@
       <c r="G59" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>25</v>
       </c>
@@ -1883,8 +2048,11 @@
       <c r="G60" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>81</v>
       </c>
@@ -1909,8 +2077,11 @@
       <c r="H62">
         <v>49.0002</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -1932,8 +2103,11 @@
       <c r="G63" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -1955,8 +2129,11 @@
       <c r="G64" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I64" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -1978,8 +2155,11 @@
       <c r="G65" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I65" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -2001,8 +2181,11 @@
       <c r="G66" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I66" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -2027,8 +2210,11 @@
       <c r="H68">
         <v>49.0002</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I68" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>82</v>
       </c>
@@ -2050,8 +2236,11 @@
       <c r="G69" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -2073,8 +2262,11 @@
       <c r="G70" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I70" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -2096,8 +2288,11 @@
       <c r="G71" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -2119,8 +2314,11 @@
       <c r="G72" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I72" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>94</v>
       </c>
@@ -2145,8 +2343,11 @@
       <c r="H74">
         <v>49.000100000000003</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I74" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>94</v>
       </c>
@@ -2157,7 +2358,7 @@
         <v>104</v>
       </c>
       <c r="D75" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E75">
         <v>31</v>
@@ -2168,8 +2369,11 @@
       <c r="G75" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I75" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>94</v>
       </c>
@@ -2180,7 +2384,7 @@
         <v>105</v>
       </c>
       <c r="D76" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E76">
         <v>31</v>
@@ -2191,28 +2395,34 @@
       <c r="G76" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I76" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C77">
         <v>255</v>
       </c>
       <c r="D77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E77">
         <v>24</v>
       </c>
       <c r="F77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G77" t="s">
-        <v>96</v>
+        <v>113</v>
+      </c>
+      <c r="I77" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>